<commit_message>
Update memory schematic & parts
</commit_message>
<xml_diff>
--- a/Hardware/parts.xlsx
+++ b/Hardware/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xia_t\Desktop\Projects\riscv\rv32i_dev\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC457F-D123-4C18-B570-763C98C23153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2181DC8-DBBD-46E3-979A-53F3EAC09171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
+    <workbookView xWindow="13335" yWindow="2715" windowWidth="11985" windowHeight="11385" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,10 +109,10 @@
     <t>https://datasheet.lcsc.com/lcsc/1912141436_ISSI-Integrated-Silicon-Solution-IS61C5128AS-25QLI_C443416.pdf</t>
   </si>
   <si>
-    <t>74HC138PW</t>
-  </si>
-  <si>
     <t>https://datasheet.lcsc.com/lcsc/1809191939_Nexperia-74HC138PW-118_C47455.pdf</t>
+  </si>
+  <si>
+    <t>74HC138PWR</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,10 +576,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add schmitt trigger to parts list
</commit_message>
<xml_diff>
--- a/Hardware/parts.xlsx
+++ b/Hardware/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xia_t\Desktop\Projects\riscv\rv32i_dev\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2181DC8-DBBD-46E3-979A-53F3EAC09171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02CCB1A-B2C2-4D33-ABA3-AF8EABD969C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13335" yWindow="2715" windowWidth="11985" windowHeight="11385" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">or </t>
   </si>
@@ -58,9 +58,6 @@
     <t>Datasheet</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
     <t>https://www.ti.com/lit/ds/symlink/sn74hcs86.pdf?ts=1638720224397&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Flogic-voltage-translation%252Flogic-gates%252Fexclusive-or-xor-gates%252Fproducts.html</t>
   </si>
   <si>
@@ -113,6 +110,21 @@
   </si>
   <si>
     <t>74HC138PWR</t>
+  </si>
+  <si>
+    <t>SN74ACT14</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/sn74act14.pdf?HQS=dis-mous-null-mousermode-dsf-pf-null-wwe&amp;ts=1640459360692&amp;ref_url=https%253A%252F%252Fwww.mouser.ca%252F</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>schmitt trigger</t>
+  </si>
+  <si>
+    <t>out of stock</t>
   </si>
 </sst>
 </file>
@@ -492,17 +504,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A35180F-508E-4FA7-A440-47C76079363F}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -512,11 +523,11 @@
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -526,8 +537,8 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -537,8 +548,8 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
+      <c r="D3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -546,77 +557,92 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{D7011177-420E-4F70-A4F2-E339BDF0AEF6}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{764EE89A-0AA7-4B36-86CC-92F5E6D9DE29}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{D8819FB7-3FC6-440C-9E8F-080803227A64}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{3AD78C78-7837-40BF-BF0B-15F5320C8A2A}"/>
-    <hyperlink ref="C6" r:id="rId5" xr:uid="{B92E909B-923A-4852-8EDA-D223CA778BA6}"/>
-    <hyperlink ref="C8" r:id="rId6" xr:uid="{8B004D3D-8B69-421D-91DD-9DD2BAF0DC4E}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{2866A33E-D6F7-47DB-8C73-2D5EDC622132}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{D7011177-420E-4F70-A4F2-E339BDF0AEF6}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{764EE89A-0AA7-4B36-86CC-92F5E6D9DE29}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{D8819FB7-3FC6-440C-9E8F-080803227A64}"/>
+    <hyperlink ref="D3" r:id="rId4" xr:uid="{3AD78C78-7837-40BF-BF0B-15F5320C8A2A}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{B92E909B-923A-4852-8EDA-D223CA778BA6}"/>
+    <hyperlink ref="D9" r:id="rId6" xr:uid="{8B004D3D-8B69-421D-91DD-9DD2BAF0DC4E}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{2866A33E-D6F7-47DB-8C73-2D5EDC622132}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
Add register, counter, rom to parts list
</commit_message>
<xml_diff>
--- a/Hardware/parts.xlsx
+++ b/Hardware/parts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xia_t\Desktop\Projects\riscv\rv32i_dev\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02CCB1A-B2C2-4D33-ABA3-AF8EABD969C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A837E690-9ED4-4B83-B9ED-4A80D5877AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">or </t>
   </si>
@@ -125,6 +125,36 @@
   </si>
   <si>
     <t>out of stock</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/sn74hc161.pdf?HQS=dis-mous-null-mousermode-dsf-pf-null-wwe&amp;ts=1640512735338</t>
+  </si>
+  <si>
+    <t>4 bit only</t>
+  </si>
+  <si>
+    <t>MT29F8G08ABACA</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/1912111437_Micron-Tech-MT29F8G08ABACAWP-IT-C_C400999.pdf</t>
+  </si>
+  <si>
+    <t>same addr and i/o</t>
+  </si>
+  <si>
+    <t>AT28C64</t>
+  </si>
+  <si>
+    <t>https://ww1.microchip.com/downloads/en/DeviceDoc/doc0270.pdf</t>
+  </si>
+  <si>
+    <t>SN74HC161DR</t>
+  </si>
+  <si>
+    <t>https://www.ti.com/lit/ds/symlink/sn74hct574.pdf?ts=1640527510946&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FSN74HCT574%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dasc-int-lvt-prodfolderdynamic-cpc-pf-google-wwe%2526utm_content%253Dprodfolddynamic%2526ds_k%253DDYNAMIC%2BSEARCH%2BADS%2526DCM%253Dyes%2526gclid%253DCj0KCQiAwqCOBhCdARIsAEPyW9k3RiLEWJBSyZsyJfcgBFzijBS9H81wBqR6zBzhKHt4lWJ7ZB4cynsaAolWEALw_wcB%2526gclsrc%253Daw.ds</t>
+  </si>
+  <si>
+    <t>SN74HCT574PWR</t>
   </si>
 </sst>
 </file>
@@ -504,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A35180F-508E-4FA7-A440-47C76079363F}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C15" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,15 +653,47 @@
       <c r="A10" t="s">
         <v>19</v>
       </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -643,8 +705,11 @@
     <hyperlink ref="D7" r:id="rId5" xr:uid="{B92E909B-923A-4852-8EDA-D223CA778BA6}"/>
     <hyperlink ref="D9" r:id="rId6" xr:uid="{8B004D3D-8B69-421D-91DD-9DD2BAF0DC4E}"/>
     <hyperlink ref="D8" r:id="rId7" xr:uid="{2866A33E-D6F7-47DB-8C73-2D5EDC622132}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{866B1158-6211-47E6-B6E8-87B86690B11A}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{4322824B-C341-4049-B67C-3ECA8B170F59}"/>
+    <hyperlink ref="D12" r:id="rId10" display="https://www.ti.com/lit/ds/symlink/sn74hct574.pdf?ts=1640527510946&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FSN74HCT574%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dasc-int-lvt-prodfolderdynamic-cpc-pf-google-wwe%2526utm_content%253Dprodfolddynamic%2526ds_k%253DDYNAMIC%2BSEARCH%2BADS%2526DCM%253Dyes%2526gclid%253DCj0KCQiAwqCOBhCdARIsAEPyW9k3RiLEWJBSyZsyJfcgBFzijBS9H81wBqR6zBzhKHt4lWJ7ZB4cynsaAolWEALw_wcB%2526gclsrc%253Daw.ds" xr:uid="{8552FB53-0F54-4CB2-8112-C05C3260AC9C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Altium Design Files
</commit_message>
<xml_diff>
--- a/Hardware/parts.xlsx
+++ b/Hardware/parts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xia_t\Desktop\Projects\riscv\rv32i_dev\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC058BB-7EB8-4A65-8A08-FB8B6750C030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E504E8-C189-476E-B489-43F0550DA277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17130" yWindow="3090" windowWidth="11985" windowHeight="11385" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
+    <workbookView xWindow="14145" yWindow="2790" windowWidth="11985" windowHeight="11385" xr2:uid="{49D5D7AF-B51C-490D-9A33-2F59ECB46A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">or </t>
   </si>
@@ -173,6 +173,45 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/1809051921_STMicroelectronics-M95M01-RMN6TP_C111166.pdf</t>
+  </si>
+  <si>
+    <t>2mbit</t>
+  </si>
+  <si>
+    <t>w25q16jvsniq</t>
+  </si>
+  <si>
+    <t>https://item.szlcsc.com/116655.html</t>
+  </si>
+  <si>
+    <t>1v2 reg</t>
+  </si>
+  <si>
+    <t>md5112</t>
+  </si>
+  <si>
+    <t>https://item.szlcsc.com/998676.html</t>
+  </si>
+  <si>
+    <t>lm317a</t>
+  </si>
+  <si>
+    <t>xc6206p12</t>
+  </si>
+  <si>
+    <t>https://atta.szlcsc.com//upload/public/pdf/source/20130801/1457706628791.pdf</t>
+  </si>
+  <si>
+    <t>ld1117s12</t>
+  </si>
+  <si>
+    <t>diode</t>
+  </si>
+  <si>
+    <t>1N5819WS</t>
+  </si>
+  <si>
+    <t>https://atta.szlcsc.com//upload/public/pdf/source/20180614/C191023_3C6A6398B911F3A4C23E7538EE054643.pdf</t>
   </si>
 </sst>
 </file>
@@ -552,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A35180F-508E-4FA7-A440-47C76079363F}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,6 +773,57 @@
       </c>
       <c r="D16" s="2" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -749,8 +839,12 @@
     <hyperlink ref="D10" r:id="rId9" xr:uid="{4322824B-C341-4049-B67C-3ECA8B170F59}"/>
     <hyperlink ref="D12" r:id="rId10" display="https://www.ti.com/lit/ds/symlink/sn74hct574.pdf?ts=1640527510946&amp;ref_url=https%253A%252F%252Fwww.ti.com%252Fproduct%252FSN74HCT574%253Futm_source%253Dgoogle%2526utm_medium%253Dcpc%2526utm_campaign%253Dasc-int-lvt-prodfolderdynamic-cpc-pf-google-wwe%2526utm_content%253Dprodfolddynamic%2526ds_k%253DDYNAMIC%2BSEARCH%2BADS%2526DCM%253Dyes%2526gclid%253DCj0KCQiAwqCOBhCdARIsAEPyW9k3RiLEWJBSyZsyJfcgBFzijBS9H81wBqR6zBzhKHt4lWJ7ZB4cynsaAolWEALw_wcB%2526gclsrc%253Daw.ds" xr:uid="{8552FB53-0F54-4CB2-8112-C05C3260AC9C}"/>
     <hyperlink ref="D16" r:id="rId11" xr:uid="{B21B6CEA-BFE2-446E-8A69-F49D269C8ECE}"/>
+    <hyperlink ref="D17" r:id="rId12" xr:uid="{20698A34-4FB4-4270-A5CF-57AC0BA331C8}"/>
+    <hyperlink ref="D18" r:id="rId13" xr:uid="{96AFCB1B-7C15-453C-9E0A-5754350C472E}"/>
+    <hyperlink ref="D20" r:id="rId14" xr:uid="{C643E4E6-4C35-4937-B028-7728A7BDA26B}"/>
+    <hyperlink ref="D22" r:id="rId15" xr:uid="{606D15AA-76C2-4338-B8AF-3EC2D52976B9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>